<commit_message>
Moved PMTCT FO to SMI dataset
</commit_message>
<xml_diff>
--- a/conf/param.xlsx
+++ b/conf/param.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asamuel/Projects/ccs-datim-data-import/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5147E5F-37EA-9542-ACB7-AEE30DFC9459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76369C1D-2820-EF41-9218-EA22F2F2D6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16260" yWindow="520" windowWidth="18680" windowHeight="19440" firstSheet="3" activeTab="3" xr2:uid="{96DDD155-47A8-3046-A85A-1FDBF652BB50}"/>
+    <workbookView xWindow="16260" yWindow="620" windowWidth="18680" windowHeight="19440" firstSheet="3" activeTab="6" xr2:uid="{96DDD155-47A8-3046-A85A-1FDBF652BB50}"/>
   </bookViews>
   <sheets>
     <sheet name="mer_datasets_names" sheetId="1" r:id="rId1"/>
@@ -1592,7 +1592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2990364B-7183-FE40-81AB-376DD313779B}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1845,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2608F92-B839-4647-A85A-A1A0390AF090}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1973,10 +1973,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1984,7 +1984,7 @@
         <v>104</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1992,7 +1992,7 @@
         <v>104</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2000,15 +2000,15 @@
         <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2016,7 +2016,7 @@
         <v>115</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2024,7 +2024,7 @@
         <v>115</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2032,15 +2032,15 @@
         <v>115</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2048,23 +2048,23 @@
         <v>120</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>123</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>125</v>
+      <c r="C26" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2072,7 +2072,7 @@
         <v>123</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2080,7 +2080,7 @@
         <v>123</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>